<commit_message>
remove many unneccessary files
</commit_message>
<xml_diff>
--- a/20191021/result/test/posts.xlsx
+++ b/20191021/result/test/posts.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\part_time_jobs\crawler\facebook\facebook\20191021\result\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace_python\facebook-data\20191021\result\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E30CCEBA-0D8D-4467-AE2D-978311A612E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAA7CC49-E285-4FBA-8656-26341EB54111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="post" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="181029" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -3271,7 +3271,9 @@
   </sheetPr>
   <dimension ref="A1:D323"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="C327" sqref="C327"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>